<commit_message>
update section name 2LCRCP -> 2LCRCP-HOU
</commit_message>
<xml_diff>
--- a/special_sections/two_lift_CRCP/excel_files/two_lift_section_info.xlsx
+++ b/special_sections/two_lift_CRCP/excel_files/two_lift_section_info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://texastechuniversity-my.sharepoint.com/personal/samuel_alalade_ttu_edu/Documents/Research/PhD/0-7147/Tasks/Task 9/Shared FIles/rpdb/sections_info/special_sections/two_lift_section/excel_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\TxRPDB\rpdb-data-v3.0\special_sections\two_lift_CRCP\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_034160E4F613C846C91280FB1636CCDC7552B6EB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90274DCA-29C8-4DD7-9D24-5F8682FFE65D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A7AF062-DFA5-4580-9559-660B3A19003F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -103,9 +103,6 @@
     <t>Two Lift Section</t>
   </si>
   <si>
-    <t>2LCRCP</t>
-  </si>
-  <si>
     <t>US59</t>
   </si>
   <si>
@@ -122,6 +119,9 @@
   </si>
   <si>
     <t>Fort Bend</t>
+  </si>
+  <si>
+    <t>2LCRCP-HOU</t>
   </si>
 </sst>
 </file>
@@ -492,7 +492,7 @@
   <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,25 +582,25 @@
         <v>26</v>
       </c>
       <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
         <v>27</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>28</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>29</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>30</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" t="s">
         <v>31</v>
-      </c>
-      <c r="G2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I2" t="s">
-        <v>32</v>
       </c>
       <c r="L2">
         <v>2017</v>

</xml_diff>